<commit_message>
Completed basic working version of sample form
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA47028F-2C9A-2544-A05F-D7F2EE55C499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EB91F8-93E3-E34F-A265-34444E0F5CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28080" yWindow="1380" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="404">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2621,13 +2621,91 @@
     <t>select_one truefalse</t>
   </si>
   <si>
-    <t>Birds lay eggs.</t>
-  </si>
-  <si>
     <t>long_list</t>
   </si>
   <si>
-    <t>custom-timed-field-list(labels='Birds lay eggs.|Chickens have pencils.|Six is a shape.|A house has a door.|Football is a game.|Men can walk.|We eat paper.|Bees make bread.|Cars have tires.|Ball is a color.|Bees make honey.|A mouse has a door.|We eat food.|Red is a color.|Chickens have feathers.|Boats have tires.|Six is a number.|Desks can walk.|Dogs lay eggs.|Football is a meal.')</t>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>long_list_data</t>
+  </si>
+  <si>
+    <t>plug-in-metadata(${long_list})</t>
+  </si>
+  <si>
+    <t>This field has no parameters defined other than the labels.</t>
+  </si>
+  <si>
+    <t>long_list_time_left</t>
+  </si>
+  <si>
+    <t>long_list_ans</t>
+  </si>
+  <si>
+    <t>num_labels</t>
+  </si>
+  <si>
+    <t>${num_labels}</t>
+  </si>
+  <si>
+    <t>long_list_answer</t>
+  </si>
+  <si>
+    <t>long_list_label</t>
+  </si>
+  <si>
+    <t>choice-label(${long_list}, ${long_list_answer})</t>
+  </si>
+  <si>
+    <t>ans_disp</t>
+  </si>
+  <si>
+    <t>join(linebreak(), ${long_list_label})</t>
+  </si>
+  <si>
+    <t>labels</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels})</t>
+  </si>
+  <si>
+    <t>'Birds lay eggs.|Chickens have pencils.|Six is a shape.|A house has a door.|Football is a game.|Men can walk.|We eat paper.|Bees make bread.|Cars have tires.|Ball is a color.|Bees make honey.|A mouse has a door.|We eat food.|Red is a color.|Chickens have feathers.|Boats have tires.|Six is a number.|Desks can walk.|Dogs lay eggs.|Football is a meal.'</t>
+  </si>
+  <si>
+    <t>no_advance</t>
+  </si>
+  <si>
+    <t>This field will not auto-advance, but it will block input after time runs out.</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, advance=0)</t>
+  </si>
+  <si>
+    <t>long_list_disp</t>
+  </si>
+  <si>
+    <t>${ans_disp}</t>
+  </si>
+  <si>
+    <t>no_block</t>
+  </si>
+  <si>
+    <t>This field will not auto-advance, nor will it will block input after time runs out.</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, advance=0, block=0)</t>
+  </si>
+  <si>
+    <t>Retrieve selected choice labels</t>
+  </si>
+  <si>
+    <t>count-items('|', ${long_list_data}) - 1</t>
+  </si>
+  <si>
+    <t>item-at('|', ${long_list_data}, index())</t>
+  </si>
+  <si>
+    <t>item-at('|', ${long_list_data}, 0)</t>
   </si>
 </sst>
 </file>
@@ -3076,7 +3154,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3226,6 +3304,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4778,16 +4857,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29" style="9" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" style="9" customWidth="1"/>
     <col min="3" max="3" width="30.5" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="11" bestFit="1" customWidth="1"/>
@@ -4978,24 +5059,168 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="N12" s="65" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>376</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="C14" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>377</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>399</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I1048576 F1:F1048576 B1:C1048576">
+  <conditionalFormatting sqref="I1:I1048576 B1:C1048576 F1:F1048576">
     <cfRule type="expression" dxfId="133" priority="49" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
@@ -5005,7 +5230,7 @@
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:D1048576">
+  <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
     <cfRule type="expression" dxfId="131" priority="43" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
@@ -5020,12 +5245,12 @@
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:C1048576">
+  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
     <cfRule type="expression" dxfId="128" priority="34" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:B1048576">
+  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
     <cfRule type="expression" dxfId="127" priority="24" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
@@ -5046,12 +5271,12 @@
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:C1048576">
+  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
     <cfRule type="expression" dxfId="122" priority="14" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:C1048576">
+  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
     <cfRule type="expression" dxfId="121" priority="10" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
@@ -5125,7 +5350,7 @@
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:B1048576">
+  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
     <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
@@ -5142,7 +5367,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5227,7 +5452,15 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
+      <c r="A7" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="B7" s="15">
+        <v>-99</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
@@ -5315,7 +5548,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2006181858</v>
+        <v>2006181941</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Updated sample form with example of "nochange"
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EB91F8-93E3-E34F-A265-34444E0F5CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F922EE-5AB7-9847-A0B0-7292A0E4E17E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="407">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2706,6 +2706,15 @@
   </si>
   <si>
     <t>item-at('|', ${long_list_data}, 0)</t>
+  </si>
+  <si>
+    <t>block_row</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, advance=0, block=0 nochange=1)</t>
+  </si>
+  <si>
+    <t>This field will block a row after a choice has been selected. It will also not auto-advance, nor will it will block input after time runs out.</t>
   </si>
 </sst>
 </file>
@@ -3270,6 +3279,8 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3303,8 +3314,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -3416,7 +3425,277 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="134">
+  <dxfs count="169">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6D9E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4857,13 +5136,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5068,7 +5347,7 @@
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
-      <c r="N12" s="65" t="s">
+      <c r="N12" s="54" t="s">
         <v>391</v>
       </c>
     </row>
@@ -5217,142 +5496,291 @@
         <v>399</v>
       </c>
     </row>
+    <row r="27" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>405</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I1048576 B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="133" priority="49" stopIfTrue="1">
+  <conditionalFormatting sqref="I1:I26 B1:C26 F1:F26 F28:F1048576 B28:C1048576 I28:I1048576">
+    <cfRule type="expression" dxfId="168" priority="84" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1048576 I1:I1048576 B1:C1048576">
-    <cfRule type="expression" dxfId="132" priority="46" stopIfTrue="1">
+  <conditionalFormatting sqref="O1:O26 I1:I26 B1:C26 B28:C1048576 I28:I1048576 O28:O1048576">
+    <cfRule type="expression" dxfId="167" priority="81" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="131" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D26 F1:F26 F28:F1048576 B28:D1048576">
+    <cfRule type="expression" dxfId="166" priority="78" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H1048576 B1:D1048576">
-    <cfRule type="expression" dxfId="130" priority="41" stopIfTrue="1">
+  <conditionalFormatting sqref="G1:H26 B1:D26 B28:D1048576 G28:H1048576">
+    <cfRule type="expression" dxfId="165" priority="76" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H1048576 B1:D1048576">
-    <cfRule type="expression" dxfId="129" priority="39" stopIfTrue="1">
+  <conditionalFormatting sqref="G1:H26 B1:D26 B28:D1048576 G28:H1048576">
+    <cfRule type="expression" dxfId="164" priority="74" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="128" priority="34" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C26 F1:F26 F28:F1048576 B28:C1048576">
+    <cfRule type="expression" dxfId="163" priority="69" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="127" priority="24" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B26 F1:F26 F28:F1048576 B28:B1048576">
+    <cfRule type="expression" dxfId="162" priority="59" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="126" priority="18" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C26 B28:C1048576">
+    <cfRule type="expression" dxfId="161" priority="53" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="55" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="57" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="123" priority="16" stopIfTrue="1">
+  <conditionalFormatting sqref="N1:N26 B1:B26 B28:B1048576 N28:N1048576">
+    <cfRule type="expression" dxfId="158" priority="51" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="122" priority="14" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C26 F1:F26 F28:F1048576 B28:C1048576">
+    <cfRule type="expression" dxfId="157" priority="49" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="121" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C26 F1:F26 F28:F1048576 B28:C1048576">
+    <cfRule type="expression" dxfId="156" priority="45" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="120" priority="8" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C26 B28:C1048576">
+    <cfRule type="expression" dxfId="155" priority="43" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W1048576">
-    <cfRule type="expression" dxfId="119" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="A1:W26 A28:W1048576">
+    <cfRule type="expression" dxfId="154" priority="37" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="40" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="44" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="46" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="50" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="54" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="56" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="58" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="60" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="63" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="70" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="75" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="77" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="79" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="80" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="82" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="83" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="85" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B26 B28:B1048576">
+    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B26 F1:F26 F28:F1048576 B28:B1048576">
+    <cfRule type="expression" dxfId="134" priority="36" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27 B27:C27 F27">
+    <cfRule type="expression" dxfId="34" priority="34" stopIfTrue="1">
+      <formula>$A27="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O27 I27 B27:C27">
+    <cfRule type="expression" dxfId="33" priority="31" stopIfTrue="1">
+      <formula>$A27="begin repeat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:D27 F27">
+    <cfRule type="expression" dxfId="32" priority="28" stopIfTrue="1">
+      <formula>$A27="text"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27:H27 B27:D27">
+    <cfRule type="expression" dxfId="31" priority="26" stopIfTrue="1">
+      <formula>$A27="integer"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27:H27 B27:D27">
+    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+      <formula>$A27="decimal"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:C27 F27">
+    <cfRule type="expression" dxfId="29" priority="22" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A27, 16)="select_multiple ", LEN($A27)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A27, 17)))), AND(LEFT($A27, 11)="select_one ", LEN($A27)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A27, 12)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27 F27">
+    <cfRule type="expression" dxfId="28" priority="19" stopIfTrue="1">
+      <formula>OR($A27="audio audit", $A27="text audit", $A27="speed violations count", $A27="speed violations list", $A27="speed violations audit")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:C27">
+    <cfRule type="expression" dxfId="27" priority="13" stopIfTrue="1">
+      <formula>$A27="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="15" stopIfTrue="1">
+      <formula>$A27="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
+      <formula>OR($A27="geopoint", $A27="geoshape", $A27="geotrace")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N27 B27">
+    <cfRule type="expression" dxfId="24" priority="11" stopIfTrue="1">
+      <formula>OR($A27="calculate", $A27="calculate_here")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:C27 F27">
+    <cfRule type="expression" dxfId="23" priority="9" stopIfTrue="1">
+      <formula>OR($A27="date", $A27="datetime")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:C27 F27">
+    <cfRule type="expression" dxfId="22" priority="7" stopIfTrue="1">
+      <formula>$A27="image"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:C27">
+    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
+      <formula>OR($A27="audio", $A27="video")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:W27">
+    <cfRule type="expression" dxfId="20" priority="2" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A27, 14)="sensor_stream ", LEN($A27)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A27, 15)))), AND(LEFT($A27, 17)="sensor_statistic ", LEN($A27)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A27, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
+      <formula>$A27="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="6" stopIfTrue="1">
+      <formula>OR($A27="audio", $A27="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="8" stopIfTrue="1">
+      <formula>$A27="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="10" stopIfTrue="1">
+      <formula>OR($A27="date", $A27="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="12" stopIfTrue="1">
+      <formula>OR($A27="calculate", $A27="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="14" stopIfTrue="1">
+      <formula>$A27="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
+      <formula>$A27="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="18" stopIfTrue="1">
+      <formula>OR($A27="geopoint", $A27="geoshape", $A27="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
+      <formula>OR($A27="audio audit", $A27="text audit", $A27="speed violations count", $A27="speed violations list", $A27="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="21" stopIfTrue="1">
+      <formula>OR($A27="username", $A27="phonenumber", $A27="start", $A27="end", $A27="deviceid", $A27="subscriberid", $A27="simserial", $A27="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A27, 16)="select_multiple ", LEN($A27)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A27, 17)))), AND(LEFT($A27, 11)="select_one ", LEN($A27)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A27, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="25" stopIfTrue="1">
+      <formula>$A27="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="27" stopIfTrue="1">
+      <formula>$A27="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="29" stopIfTrue="1">
+      <formula>$A27="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="30" stopIfTrue="1">
+      <formula>$A27="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="32" stopIfTrue="1">
+      <formula>$A27="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="33" stopIfTrue="1">
+      <formula>$A27="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="35" stopIfTrue="1">
+      <formula>$A27="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+      <formula>$A27="comments"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27 F27">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A27, 14)="sensor_stream ", LEN($A27)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A27, 15)))), AND(LEFT($A27, 17)="sensor_statistic ", LEN($A27)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A27, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -5425,7 +5853,7 @@
       <c r="B4" s="15">
         <v>1</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="53" t="s">
         <v>371</v>
       </c>
     </row>
@@ -5436,7 +5864,7 @@
       <c r="B5" s="15">
         <v>0</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="53" t="s">
         <v>372</v>
       </c>
     </row>
@@ -5490,7 +5918,7 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:H2000">
-    <cfRule type="expression" dxfId="98" priority="1">
+    <cfRule type="expression" dxfId="133" priority="1">
       <formula>NOT($A2=$A1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5548,7 +5976,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2006181941</v>
+        <v>2006241812</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>
@@ -5583,22 +6011,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:30" s="33" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -5792,10 +6220,10 @@
       <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="61" t="s">
         <v>276</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
@@ -6140,7 +6568,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>102</v>
       </c>
@@ -8585,10 +9013,10 @@
       <c r="AD81" s="43"/>
     </row>
     <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="60" t="s">
+      <c r="A83" s="62" t="s">
         <v>272</v>
       </c>
-      <c r="B83" s="61"/>
+      <c r="B83" s="63"/>
       <c r="C83" s="26"/>
       <c r="D83" s="25"/>
       <c r="E83" s="30"/>
@@ -9384,348 +9812,348 @@
     <mergeCell ref="A83:B83"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9748,20 +10176,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="56"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="60"/>
     </row>
     <row r="4" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -9836,28 +10264,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="63"/>
+      <c r="B1" s="65"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>

</xml_diff>

<commit_message>
Added missing comma in parameter list
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F922EE-5AB7-9847-A0B0-7292A0E4E17E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4BC5B8-CD88-0646-8094-4714A352E97E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2711,10 +2711,10 @@
     <t>block_row</t>
   </si>
   <si>
-    <t>custom-timed-field-list(labels=${labels}, advance=0, block=0 nochange=1)</t>
-  </si>
-  <si>
     <t>This field will block a row after a choice has been selected. It will also not auto-advance, nor will it will block input after time runs out.</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, advance=0, block=0, nochange=1)</t>
   </si>
 </sst>
 </file>
@@ -5142,7 +5142,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5504,10 +5504,10 @@
         <v>404</v>
       </c>
       <c r="C27" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>406</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -5976,7 +5976,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2006241812</v>
+        <v>2006241822</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Removed requirement for "pass" value to be a choice value
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B9C165-624D-4B47-8C05-1E4B63C80D0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FC8044-DAA0-1E42-BE13-33784DC6ED6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28000" yWindow="760" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27520" yWindow="560" windowWidth="25000" windowHeight="15540" tabRatio="534" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="435">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2633,9 +2633,6 @@
     <t>plug-in-metadata(${long_list})</t>
   </si>
   <si>
-    <t>This field has no parameters defined other than the labels.</t>
-  </si>
-  <si>
     <t>long_list_time_left</t>
   </si>
   <si>
@@ -2651,24 +2648,15 @@
     <t>long_list_answer</t>
   </si>
   <si>
-    <t>long_list_label</t>
-  </si>
-  <si>
     <t>choice-label(${long_list}, ${long_list_answer})</t>
   </si>
   <si>
     <t>ans_disp</t>
   </si>
   <si>
-    <t>join(linebreak(), ${long_list_label})</t>
-  </si>
-  <si>
     <t>labels</t>
   </si>
   <si>
-    <t>custom-timed-field-list(labels=${labels})</t>
-  </si>
-  <si>
     <t>'Birds lay eggs.|Chickens have pencils.|Six is a shape.|A house has a door.|Football is a game.|Men can walk.|We eat paper.|Bees make bread.|Cars have tires.|Ball is a color.|Bees make honey.|A mouse has a door.|We eat food.|Red is a color.|Chickens have feathers.|Boats have tires.|Six is a number.|Desks can walk.|Dogs lay eggs.|Football is a meal.'</t>
   </si>
   <si>
@@ -2684,9 +2672,6 @@
     <t>long_list_disp</t>
   </si>
   <si>
-    <t>${ans_disp}</t>
-  </si>
-  <si>
     <t>no_block</t>
   </si>
   <si>
@@ -2700,12 +2685,6 @@
   </si>
   <si>
     <t>count-items('|', ${long_list_data}) - 1</t>
-  </si>
-  <si>
-    <t>item-at('|', ${long_list_data}, index())</t>
-  </si>
-  <si>
-    <t>item-at('|', ${long_list_data}, 0)</t>
   </si>
   <si>
     <t>block_row</t>
@@ -2783,6 +2762,46 @@
   </si>
   <si>
     <t>This field will not auto-advance, and it will only block input when each row has been completed.</t>
+  </si>
+  <si>
+    <t>Number of rows. Subtract 1, because the first piece of data is for timing.</t>
+  </si>
+  <si>
+    <t>There were ${long_list_time_left} milliseconds remaining.
+${ans_disp}</t>
+  </si>
+  <si>
+    <t>long_list_result_row</t>
+  </si>
+  <si>
+    <t>long_list_index</t>
+  </si>
+  <si>
+    <t>item-at('|', ${long_list_data}, ${long_list_index})</t>
+  </si>
+  <si>
+    <t>item-at('|', ${labels}, ${long_list_index} - 1)</t>
+  </si>
+  <si>
+    <t>join(linebreak(), ${long_list_result_row})</t>
+  </si>
+  <si>
+    <t>long_list_choice_label</t>
+  </si>
+  <si>
+    <t>long_list_row_label</t>
+  </si>
+  <si>
+    <t>concat(${long_list_index}, '. ', ${long_list_row_label}, ' ', ${long_list_choice_label})</t>
+  </si>
+  <si>
+    <t>selected-at(item-at('|', ${long_list_data}, 0), 0)</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, duration=20)</t>
+  </si>
+  <si>
+    <t>This field has no parameters defined other than the labels and the duration.</t>
   </si>
 </sst>
 </file>
@@ -3493,7 +3512,23 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="169">
+  <dxfs count="170">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5204,13 +5239,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5411,12 +5446,12 @@
         <v>148</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="N12" s="54" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
@@ -5428,15 +5463,15 @@
         <v>42</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="9" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5444,21 +5479,21 @@
         <v>96</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="9" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="34" x14ac:dyDescent="0.2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>374</v>
       </c>
@@ -5466,16 +5501,16 @@
         <v>375</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>379</v>
+        <v>434</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>390</v>
+        <v>433</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -5494,21 +5529,24 @@
         <v>148</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>148</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>422</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -5516,13 +5554,13 @@
         <v>163</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -5530,10 +5568,10 @@
         <v>148</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>384</v>
+        <v>425</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>402</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -5541,18 +5579,21 @@
         <v>148</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>386</v>
+        <v>426</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>381</v>
+        <v>429</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -5560,74 +5601,62 @@
         <v>148</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>387</v>
+        <v>430</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="N27" s="9" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="289" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+      <c r="B28" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="289" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>424</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="68" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>374</v>
-      </c>
       <c r="B30" s="9" t="s">
-        <v>404</v>
+        <v>417</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>405</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>406</v>
+        <v>419</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -5635,300 +5664,342 @@
         <v>374</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>425</v>
+        <v>388</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>428</v>
+        <v>389</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>414</v>
+        <v>374</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>415</v>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I29 B1:C29 F1:F29 F32:F1048576 B32:C1048576 I32:I1048576">
-    <cfRule type="expression" dxfId="168" priority="84" stopIfTrue="1">
+  <conditionalFormatting sqref="I1:I32 B1:C32 F1:F32 F35:F1048576 B35:C1048576 I35:I1048576">
+    <cfRule type="expression" dxfId="169" priority="84" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O29 I1:I29 B1:C29 B32:C1048576 I32:I1048576 O32:O1048576">
-    <cfRule type="expression" dxfId="167" priority="81" stopIfTrue="1">
+  <conditionalFormatting sqref="O1:O32 I1:I32 B1:C32 B35:C1048576 I35:I1048576 O35:O1048576">
+    <cfRule type="expression" dxfId="168" priority="81" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D29 F1:F29 F32:F1048576 B32:D1048576">
-    <cfRule type="expression" dxfId="166" priority="78" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D32 F1:F32 F35:F1048576 B35:D1048576">
+    <cfRule type="expression" dxfId="167" priority="78" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H29 B1:D29 B32:D1048576 G32:H1048576">
-    <cfRule type="expression" dxfId="165" priority="76" stopIfTrue="1">
+  <conditionalFormatting sqref="G1:H32 B1:D32 B35:D1048576 G35:H1048576">
+    <cfRule type="expression" dxfId="166" priority="76" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H29 B1:D29 B32:D1048576 G32:H1048576">
-    <cfRule type="expression" dxfId="164" priority="74" stopIfTrue="1">
+  <conditionalFormatting sqref="G1:H32 B1:D32 B35:D1048576 G35:H1048576">
+    <cfRule type="expression" dxfId="165" priority="74" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C29 F1:F29 F32:F1048576 B32:C1048576">
-    <cfRule type="expression" dxfId="163" priority="69" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C32 F1:F32 F35:F1048576 B35:C1048576">
+    <cfRule type="expression" dxfId="164" priority="69" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B29 F1:F29 F32:F1048576 B32:B1048576">
-    <cfRule type="expression" dxfId="162" priority="59" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B32 F1:F32 F35:F1048576 B35:B1048576">
+    <cfRule type="expression" dxfId="163" priority="59" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C29 B32:C1048576">
-    <cfRule type="expression" dxfId="161" priority="53" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C32 B35:C1048576">
+    <cfRule type="expression" dxfId="162" priority="53" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="55" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="57" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N29 B1:B29 B32:B1048576 N32:N1048576">
-    <cfRule type="expression" dxfId="158" priority="51" stopIfTrue="1">
+  <conditionalFormatting sqref="N1:N32 B1:B32 B35:B1048576 N35:N1048576">
+    <cfRule type="expression" dxfId="159" priority="51" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C29 F1:F29 F32:F1048576 B32:C1048576">
-    <cfRule type="expression" dxfId="157" priority="49" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C32 F1:F32 F35:F1048576 B35:C1048576">
+    <cfRule type="expression" dxfId="158" priority="49" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C29 F1:F29 F32:F1048576 B32:C1048576">
-    <cfRule type="expression" dxfId="156" priority="45" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C32 F1:F32 F35:F1048576 B35:C1048576">
+    <cfRule type="expression" dxfId="157" priority="45" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C29 B32:C1048576">
-    <cfRule type="expression" dxfId="155" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C32 B35:C1048576">
+    <cfRule type="expression" dxfId="156" priority="43" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W29 A32:W1048576">
-    <cfRule type="expression" dxfId="154" priority="37" stopIfTrue="1">
+  <conditionalFormatting sqref="A1:W32 A35:W1048576">
+    <cfRule type="expression" dxfId="155" priority="37" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="40" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="44" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="46" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="50" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="52" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="54" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="56" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="58" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="60" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="63" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="70" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="75" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="77" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="79" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="80" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="82" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="83" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="85" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B29 B32:B1048576">
-    <cfRule type="expression" dxfId="135" priority="38" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B32 B35:B1048576">
+    <cfRule type="expression" dxfId="136" priority="38" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B29 F1:F29 F32:F1048576 B32:B1048576">
-    <cfRule type="expression" dxfId="134" priority="36" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B32 F1:F32 F35:F1048576 B35:B1048576">
+    <cfRule type="expression" dxfId="135" priority="36" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30:I31 B30:C31 F30:F31">
-    <cfRule type="expression" dxfId="133" priority="34" stopIfTrue="1">
-      <formula>$A30="begin group"</formula>
+  <conditionalFormatting sqref="I33:I34 B33:C34 F33:F34">
+    <cfRule type="expression" dxfId="134" priority="34" stopIfTrue="1">
+      <formula>$A33="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O30:O31 I30:I31 B30:C31">
-    <cfRule type="expression" dxfId="132" priority="31" stopIfTrue="1">
-      <formula>$A30="begin repeat"</formula>
+  <conditionalFormatting sqref="O33:O34 I33:I34 B33:C34">
+    <cfRule type="expression" dxfId="133" priority="31" stopIfTrue="1">
+      <formula>$A33="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:D31 F30:F31">
-    <cfRule type="expression" dxfId="131" priority="28" stopIfTrue="1">
-      <formula>$A30="text"</formula>
+  <conditionalFormatting sqref="B33:D34 F33:F34">
+    <cfRule type="expression" dxfId="132" priority="28" stopIfTrue="1">
+      <formula>$A33="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G30:H31 B30:D31">
-    <cfRule type="expression" dxfId="130" priority="26" stopIfTrue="1">
-      <formula>$A30="integer"</formula>
+  <conditionalFormatting sqref="G33:H34 B33:D34">
+    <cfRule type="expression" dxfId="131" priority="26" stopIfTrue="1">
+      <formula>$A33="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G30:H31 B30:D31">
-    <cfRule type="expression" dxfId="129" priority="24" stopIfTrue="1">
-      <formula>$A30="decimal"</formula>
+  <conditionalFormatting sqref="G33:H34 B33:D34">
+    <cfRule type="expression" dxfId="130" priority="24" stopIfTrue="1">
+      <formula>$A33="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:C31 F30:F31">
-    <cfRule type="expression" dxfId="128" priority="22" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A30, 16)="select_multiple ", LEN($A30)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A30, 17)))), AND(LEFT($A30, 11)="select_one ", LEN($A30)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A30, 12)))))</formula>
+  <conditionalFormatting sqref="B33:C34 F33:F34">
+    <cfRule type="expression" dxfId="129" priority="22" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A33, 16)="select_multiple ", LEN($A33)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A33, 17)))), AND(LEFT($A33, 11)="select_one ", LEN($A33)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A33, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B31 F30:F31">
-    <cfRule type="expression" dxfId="127" priority="19" stopIfTrue="1">
-      <formula>OR($A30="audio audit", $A30="text audit", $A30="speed violations count", $A30="speed violations list", $A30="speed violations audit")</formula>
+  <conditionalFormatting sqref="B33:B34 F33:F34">
+    <cfRule type="expression" dxfId="128" priority="19" stopIfTrue="1">
+      <formula>OR($A33="audio audit", $A33="text audit", $A33="speed violations count", $A33="speed violations list", $A33="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:C31">
-    <cfRule type="expression" dxfId="126" priority="13" stopIfTrue="1">
-      <formula>$A30="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="125" priority="15" stopIfTrue="1">
-      <formula>$A30="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="124" priority="17" stopIfTrue="1">
-      <formula>OR($A30="geopoint", $A30="geoshape", $A30="geotrace")</formula>
+  <conditionalFormatting sqref="B33:C34">
+    <cfRule type="expression" dxfId="127" priority="13" stopIfTrue="1">
+      <formula>$A33="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="15" stopIfTrue="1">
+      <formula>$A33="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="17" stopIfTrue="1">
+      <formula>OR($A33="geopoint", $A33="geoshape", $A33="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N30:N31 B30:B31">
-    <cfRule type="expression" dxfId="123" priority="11" stopIfTrue="1">
-      <formula>OR($A30="calculate", $A30="calculate_here")</formula>
+  <conditionalFormatting sqref="N33:N34 B33:B34">
+    <cfRule type="expression" dxfId="124" priority="11" stopIfTrue="1">
+      <formula>OR($A33="calculate", $A33="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:C31 F30:F31">
-    <cfRule type="expression" dxfId="122" priority="9" stopIfTrue="1">
-      <formula>OR($A30="date", $A30="datetime")</formula>
+  <conditionalFormatting sqref="B33:C34 F33:F34">
+    <cfRule type="expression" dxfId="123" priority="9" stopIfTrue="1">
+      <formula>OR($A33="date", $A33="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:C31 F30:F31">
-    <cfRule type="expression" dxfId="121" priority="7" stopIfTrue="1">
-      <formula>$A30="image"</formula>
+  <conditionalFormatting sqref="B33:C34 F33:F34">
+    <cfRule type="expression" dxfId="122" priority="7" stopIfTrue="1">
+      <formula>$A33="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:C31">
-    <cfRule type="expression" dxfId="120" priority="5" stopIfTrue="1">
-      <formula>OR($A30="audio", $A30="video")</formula>
+  <conditionalFormatting sqref="B33:C34">
+    <cfRule type="expression" dxfId="121" priority="5" stopIfTrue="1">
+      <formula>OR($A33="audio", $A33="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30:W31">
-    <cfRule type="expression" dxfId="119" priority="2" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A30, 14)="sensor_stream ", LEN($A30)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A30, 15)))), AND(LEFT($A30, 17)="sensor_statistic ", LEN($A30)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A30, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="4" stopIfTrue="1">
-      <formula>$A30="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="117" priority="6" stopIfTrue="1">
-      <formula>OR($A30="audio", $A30="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="8" stopIfTrue="1">
-      <formula>$A30="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="10" stopIfTrue="1">
-      <formula>OR($A30="date", $A30="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="114" priority="12" stopIfTrue="1">
-      <formula>OR($A30="calculate", $A30="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="113" priority="14" stopIfTrue="1">
-      <formula>$A30="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="16" stopIfTrue="1">
-      <formula>$A30="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="18" stopIfTrue="1">
-      <formula>OR($A30="geopoint", $A30="geoshape", $A30="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="20" stopIfTrue="1">
-      <formula>OR($A30="audio audit", $A30="text audit", $A30="speed violations count", $A30="speed violations list", $A30="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="21" stopIfTrue="1">
-      <formula>OR($A30="username", $A30="phonenumber", $A30="start", $A30="end", $A30="deviceid", $A30="subscriberid", $A30="simserial", $A30="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="108" priority="23" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A30, 16)="select_multiple ", LEN($A30)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A30, 17)))), AND(LEFT($A30, 11)="select_one ", LEN($A30)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A30, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="25" stopIfTrue="1">
-      <formula>$A30="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="27" stopIfTrue="1">
-      <formula>$A30="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="29" stopIfTrue="1">
-      <formula>$A30="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="30" stopIfTrue="1">
-      <formula>$A30="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="32" stopIfTrue="1">
-      <formula>$A30="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="33" stopIfTrue="1">
-      <formula>$A30="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="101" priority="35" stopIfTrue="1">
-      <formula>$A30="begin group"</formula>
+  <conditionalFormatting sqref="A33:W34">
+    <cfRule type="expression" dxfId="120" priority="2" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A33, 14)="sensor_stream ", LEN($A33)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A33, 15)))), AND(LEFT($A33, 17)="sensor_statistic ", LEN($A33)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A33, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="119" priority="4" stopIfTrue="1">
+      <formula>$A33="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="6" stopIfTrue="1">
+      <formula>OR($A33="audio", $A33="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="8" stopIfTrue="1">
+      <formula>$A33="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="10" stopIfTrue="1">
+      <formula>OR($A33="date", $A33="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="12" stopIfTrue="1">
+      <formula>OR($A33="calculate", $A33="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="14" stopIfTrue="1">
+      <formula>$A33="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
+      <formula>$A33="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="18" stopIfTrue="1">
+      <formula>OR($A33="geopoint", $A33="geoshape", $A33="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="20" stopIfTrue="1">
+      <formula>OR($A33="audio audit", $A33="text audit", $A33="speed violations count", $A33="speed violations list", $A33="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="21" stopIfTrue="1">
+      <formula>OR($A33="username", $A33="phonenumber", $A33="start", $A33="end", $A33="deviceid", $A33="subscriberid", $A33="simserial", $A33="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="23" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A33, 16)="select_multiple ", LEN($A33)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A33, 17)))), AND(LEFT($A33, 11)="select_one ", LEN($A33)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A33, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="25" stopIfTrue="1">
+      <formula>$A33="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="27" stopIfTrue="1">
+      <formula>$A33="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="29" stopIfTrue="1">
+      <formula>$A33="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="30" stopIfTrue="1">
+      <formula>$A33="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="32" stopIfTrue="1">
+      <formula>$A33="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="33" stopIfTrue="1">
+      <formula>$A33="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="35" stopIfTrue="1">
+      <formula>$A33="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B31">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
-      <formula>$A30="comments"</formula>
+  <conditionalFormatting sqref="B33:B34">
+    <cfRule type="expression" dxfId="101" priority="3" stopIfTrue="1">
+      <formula>$A33="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B31 F30:F31">
-    <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A30, 14)="sensor_stream ", LEN($A30)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A30, 15)))), AND(LEFT($A30, 17)="sensor_statistic ", LEN($A30)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A30, 18)))))</formula>
+  <conditionalFormatting sqref="B33:B34 F33:F34">
+    <cfRule type="expression" dxfId="100" priority="1" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A33, 14)="sensor_stream ", LEN($A33)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A33, 15)))), AND(LEFT($A33, 17)="sensor_statistic ", LEN($A33)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A33, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -5939,9 +6010,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -6040,74 +6111,68 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B8" s="15">
         <v>1</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B9" s="15">
         <v>2</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B10" s="15">
         <v>3</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B11" s="15">
         <v>4</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>407</v>
-      </c>
-      <c r="B12" s="15">
-        <v>-99</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
+      <c r="A12" s="16"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:H2000">
-    <cfRule type="expression" dxfId="98" priority="1">
+  <conditionalFormatting sqref="A2:H11 A13:H1999">
+    <cfRule type="expression" dxfId="99" priority="1">
       <formula>NOT($A2=$A1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:H12">
+    <cfRule type="expression" dxfId="0" priority="100">
+      <formula>NOT($A12=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -6164,7 +6229,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007072019</v>
+        <v>2007102002</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>
@@ -10000,348 +10065,348 @@
     <mergeCell ref="A83:B83"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated sample form with more examples of parameters
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FC8044-DAA0-1E42-BE13-33784DC6ED6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF97591-7408-324A-9C93-B89469698648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27520" yWindow="560" windowWidth="25000" windowHeight="15540" tabRatio="534" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27500" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="446">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2660,42 +2660,18 @@
     <t>'Birds lay eggs.|Chickens have pencils.|Six is a shape.|A house has a door.|Football is a game.|Men can walk.|We eat paper.|Bees make bread.|Cars have tires.|Ball is a color.|Bees make honey.|A mouse has a door.|We eat food.|Red is a color.|Chickens have feathers.|Boats have tires.|Six is a number.|Desks can walk.|Dogs lay eggs.|Football is a meal.'</t>
   </si>
   <si>
-    <t>no_advance</t>
-  </si>
-  <si>
-    <t>This field will not auto-advance, but it will block input after time runs out.</t>
-  </si>
-  <si>
-    <t>custom-timed-field-list(labels=${labels}, advance=0)</t>
-  </si>
-  <si>
     <t>long_list_disp</t>
   </si>
   <si>
     <t>no_block</t>
   </si>
   <si>
-    <t>This field will not auto-advance, nor will it will block input after time runs out.</t>
-  </si>
-  <si>
-    <t>custom-timed-field-list(labels=${labels}, advance=0, block=0)</t>
-  </si>
-  <si>
     <t>Retrieve selected choice labels</t>
   </si>
   <si>
     <t>count-items('|', ${long_list_data}) - 1</t>
   </si>
   <si>
-    <t>block_row</t>
-  </si>
-  <si>
-    <t>This field will block a row after a choice has been selected. It will also not auto-advance, nor will it will block input after time runs out.</t>
-  </si>
-  <si>
-    <t>custom-timed-field-list(labels=${labels}, advance=0, block=0, nochange=1)</t>
-  </si>
-  <si>
     <t>crops</t>
   </si>
   <si>
@@ -2714,13 +2690,7 @@
     <t>crop_list</t>
   </si>
   <si>
-    <t>Select the crops you see in each plot.</t>
-  </si>
-  <si>
     <t>select_multiple crops</t>
-  </si>
-  <si>
-    <t>custom-timed-field-list(labels='Plot 2|Plot 3|Plot 4|Plot 5|Plot 6|Plot 7|Plot 8|Plot 9|Plot 10|Plot 11|Plot 12|Plot 13|Plot 14|Plot 15|', header='Plots', duration=20, advance=0)</t>
   </si>
   <si>
     <t>startbutton</t>
@@ -2758,12 +2728,6 @@
 The next several fields will show off several of the parameters you can use. Serveral different combinations of parameters are used, but these examples are not exhausted, so feel free to combine parameters in other ways.</t>
   </si>
   <si>
-    <t>custom-timed-field-list(labels=${labels}, advance=0, required=1)</t>
-  </si>
-  <si>
-    <t>This field will not auto-advance, and it will only block input when each row has been completed.</t>
-  </si>
-  <si>
     <t>Number of rows. Subtract 1, because the first piece of data is for timing.</t>
   </si>
   <si>
@@ -2802,6 +2766,77 @@
   </si>
   <si>
     <t>This field has no parameters defined other than the labels and the duration.</t>
+  </si>
+  <si>
+    <t>auto_advance</t>
+  </si>
+  <si>
+    <t>This field will not block input after time runs out.</t>
+  </si>
+  <si>
+    <t>This field will only block input when each row has been completed.</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, duration=20, block=0)</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels='Plot 1|Plot 2|Plot 3|Plot 4|Plot 5|Plot 6|Plot 7|Plot 8|Plot 9|Plot 10|Plot 11|Plot 12|Plot 13|Plot 14|Plot 15|', header='Plots', duration=20)</t>
+  </si>
+  <si>
+    <t>This is an example of a &lt;em&gt;select_multiple&lt;/em&gt; field.&lt;br&gt;
+&lt;br&gt;
+Select the crops you see in each plot.</t>
+  </si>
+  <si>
+    <t>not_timed</t>
+  </si>
+  <si>
+    <t>This field is not timed.</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels})</t>
+  </si>
+  <si>
+    <t>no_disp</t>
+  </si>
+  <si>
+    <t>This field has a 10-second timer, but the timer is not displayed. Input will be blocked after 10 seconds.</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, duration=20, disp=0)</t>
+  </si>
+  <si>
+    <t>labels_short</t>
+  </si>
+  <si>
+    <t>'Birds lay eggs.|Chickens have pencils.|Six is a shape.|A house has a door.|Football is a game.|Men can walk.|We eat paper.|Bees make bread.|Cars have tires.|Ball is a color.|Bees make honey.|A mouse has a door.|We eat food.|Red is a color.'</t>
+  </si>
+  <si>
+    <t>not_endearly</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels_short}, duration=10, endearly=0)</t>
+  </si>
+  <si>
+    <t>nochange</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, duration=20, advance=1, unit='ms')</t>
+  </si>
+  <si>
+    <t>This field will auto-advance after time runs out. It also uses a different time unit.</t>
+  </si>
+  <si>
+    <t>In this field, the respondent cannot leave until time has run out, even if all fields have been completed. (This example field is required.)</t>
+  </si>
+  <si>
+    <t>This field will disable a row after a choice has been selected. It will not block input after time runs out.</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, duration=20, nochange=1, block=0)</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, duration=10, required=1)</t>
   </si>
 </sst>
 </file>
@@ -3512,7 +3547,746 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="170">
+  <dxfs count="135">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -3530,745 +4304,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4283,276 +4318,6 @@
           <color auto="1"/>
         </top>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D9E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5239,13 +5004,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W36"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5455,73 +5220,75 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>435</v>
+      </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:23" ht="255" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>416</v>
-      </c>
+      <c r="N13" s="54" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
-      <c r="K14" s="9" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:23" ht="255" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="9" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="9" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>434</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>412</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>377</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>378</v>
+      <c r="C17" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -5529,49 +5296,49 @@
         <v>148</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>148</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="N19" s="9" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+      <c r="C20" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B21" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="O20" s="9" t="s">
+      <c r="C21" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="O21" s="9" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -5579,10 +5346,10 @@
         <v>148</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>383</v>
+        <v>413</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>426</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -5590,10 +5357,10 @@
         <v>148</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>429</v>
+        <v>383</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>384</v>
+        <v>414</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -5601,10 +5368,10 @@
         <v>148</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>427</v>
+        <v>384</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -5612,65 +5379,62 @@
         <v>148</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>380</v>
+        <v>412</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B28" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="N27" s="9" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="68" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+      <c r="N28" s="9" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>391</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="289" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+      <c r="B29" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="289" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>417</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
-        <v>374</v>
-      </c>
       <c r="B31" s="9" t="s">
-        <v>388</v>
+        <v>407</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>390</v>
+        <v>409</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -5678,328 +5442,252 @@
         <v>374</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>392</v>
+        <v>423</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>393</v>
+        <v>441</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>374</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>398</v>
+        <v>424</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>374</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>407</v>
+        <v>374</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>405</v>
+        <v>439</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>406</v>
+        <v>443</v>
       </c>
       <c r="F36" s="9" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>408</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>431</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I32 B1:C32 F1:F32 F35:F1048576 B35:C1048576 I35:I1048576">
-    <cfRule type="expression" dxfId="169" priority="84" stopIfTrue="1">
+  <conditionalFormatting sqref="I1:I1048576 B1:C1048576 F1:F1048576">
+    <cfRule type="expression" dxfId="134" priority="84" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O32 I1:I32 B1:C32 B35:C1048576 I35:I1048576 O35:O1048576">
-    <cfRule type="expression" dxfId="168" priority="81" stopIfTrue="1">
+  <conditionalFormatting sqref="O1:O1048576 I1:I1048576 B1:C1048576">
+    <cfRule type="expression" dxfId="133" priority="81" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D32 F1:F32 F35:F1048576 B35:D1048576">
-    <cfRule type="expression" dxfId="167" priority="78" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
+    <cfRule type="expression" dxfId="132" priority="78" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H32 B1:D32 B35:D1048576 G35:H1048576">
-    <cfRule type="expression" dxfId="166" priority="76" stopIfTrue="1">
+  <conditionalFormatting sqref="G1:H1048576 B1:D1048576">
+    <cfRule type="expression" dxfId="131" priority="76" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H32 B1:D32 B35:D1048576 G35:H1048576">
-    <cfRule type="expression" dxfId="165" priority="74" stopIfTrue="1">
+  <conditionalFormatting sqref="G1:H1048576 B1:D1048576">
+    <cfRule type="expression" dxfId="130" priority="74" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C32 F1:F32 F35:F1048576 B35:C1048576">
-    <cfRule type="expression" dxfId="164" priority="69" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
+    <cfRule type="expression" dxfId="129" priority="69" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B32 F1:F32 F35:F1048576 B35:B1048576">
-    <cfRule type="expression" dxfId="163" priority="59" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
+    <cfRule type="expression" dxfId="128" priority="59" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C32 B35:C1048576">
-    <cfRule type="expression" dxfId="162" priority="53" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C1048576">
+    <cfRule type="expression" dxfId="127" priority="53" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="55" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="57" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N32 B1:B32 B35:B1048576 N35:N1048576">
-    <cfRule type="expression" dxfId="159" priority="51" stopIfTrue="1">
+  <conditionalFormatting sqref="N1:N1048576 B1:B1048576">
+    <cfRule type="expression" dxfId="124" priority="51" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C32 F1:F32 F35:F1048576 B35:C1048576">
-    <cfRule type="expression" dxfId="158" priority="49" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
+    <cfRule type="expression" dxfId="123" priority="49" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C32 F1:F32 F35:F1048576 B35:C1048576">
-    <cfRule type="expression" dxfId="157" priority="45" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
+    <cfRule type="expression" dxfId="122" priority="45" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C32 B35:C1048576">
-    <cfRule type="expression" dxfId="156" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C1048576">
+    <cfRule type="expression" dxfId="121" priority="43" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W32 A35:W1048576">
-    <cfRule type="expression" dxfId="155" priority="37" stopIfTrue="1">
+  <conditionalFormatting sqref="A1:W1048576">
+    <cfRule type="expression" dxfId="120" priority="37" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="40" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="44" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="46" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="50" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="52" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="54" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="56" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="58" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="60" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="63" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="70" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="75" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="77" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="79" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="80" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="82" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="83" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="85" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B32 B35:B1048576">
-    <cfRule type="expression" dxfId="136" priority="38" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="expression" dxfId="101" priority="38" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B32 F1:F32 F35:F1048576 B35:B1048576">
-    <cfRule type="expression" dxfId="135" priority="36" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
+    <cfRule type="expression" dxfId="100" priority="36" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33:I34 B33:C34 F33:F34">
-    <cfRule type="expression" dxfId="134" priority="34" stopIfTrue="1">
-      <formula>$A33="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O33:O34 I33:I34 B33:C34">
-    <cfRule type="expression" dxfId="133" priority="31" stopIfTrue="1">
-      <formula>$A33="begin repeat"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:D34 F33:F34">
-    <cfRule type="expression" dxfId="132" priority="28" stopIfTrue="1">
-      <formula>$A33="text"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33:H34 B33:D34">
-    <cfRule type="expression" dxfId="131" priority="26" stopIfTrue="1">
-      <formula>$A33="integer"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33:H34 B33:D34">
-    <cfRule type="expression" dxfId="130" priority="24" stopIfTrue="1">
-      <formula>$A33="decimal"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:C34 F33:F34">
-    <cfRule type="expression" dxfId="129" priority="22" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A33, 16)="select_multiple ", LEN($A33)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A33, 17)))), AND(LEFT($A33, 11)="select_one ", LEN($A33)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A33, 12)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:B34 F33:F34">
-    <cfRule type="expression" dxfId="128" priority="19" stopIfTrue="1">
-      <formula>OR($A33="audio audit", $A33="text audit", $A33="speed violations count", $A33="speed violations list", $A33="speed violations audit")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:C34">
-    <cfRule type="expression" dxfId="127" priority="13" stopIfTrue="1">
-      <formula>$A33="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="15" stopIfTrue="1">
-      <formula>$A33="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="125" priority="17" stopIfTrue="1">
-      <formula>OR($A33="geopoint", $A33="geoshape", $A33="geotrace")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N33:N34 B33:B34">
-    <cfRule type="expression" dxfId="124" priority="11" stopIfTrue="1">
-      <formula>OR($A33="calculate", $A33="calculate_here")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:C34 F33:F34">
-    <cfRule type="expression" dxfId="123" priority="9" stopIfTrue="1">
-      <formula>OR($A33="date", $A33="datetime")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:C34 F33:F34">
-    <cfRule type="expression" dxfId="122" priority="7" stopIfTrue="1">
-      <formula>$A33="image"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:C34">
-    <cfRule type="expression" dxfId="121" priority="5" stopIfTrue="1">
-      <formula>OR($A33="audio", $A33="video")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33:W34">
-    <cfRule type="expression" dxfId="120" priority="2" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A33, 14)="sensor_stream ", LEN($A33)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A33, 15)))), AND(LEFT($A33, 17)="sensor_statistic ", LEN($A33)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A33, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="119" priority="4" stopIfTrue="1">
-      <formula>$A33="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="6" stopIfTrue="1">
-      <formula>OR($A33="audio", $A33="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="117" priority="8" stopIfTrue="1">
-      <formula>$A33="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="10" stopIfTrue="1">
-      <formula>OR($A33="date", $A33="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="12" stopIfTrue="1">
-      <formula>OR($A33="calculate", $A33="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="114" priority="14" stopIfTrue="1">
-      <formula>$A33="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="113" priority="16" stopIfTrue="1">
-      <formula>$A33="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="18" stopIfTrue="1">
-      <formula>OR($A33="geopoint", $A33="geoshape", $A33="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="20" stopIfTrue="1">
-      <formula>OR($A33="audio audit", $A33="text audit", $A33="speed violations count", $A33="speed violations list", $A33="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="21" stopIfTrue="1">
-      <formula>OR($A33="username", $A33="phonenumber", $A33="start", $A33="end", $A33="deviceid", $A33="subscriberid", $A33="simserial", $A33="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="23" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A33, 16)="select_multiple ", LEN($A33)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A33, 17)))), AND(LEFT($A33, 11)="select_one ", LEN($A33)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A33, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="108" priority="25" stopIfTrue="1">
-      <formula>$A33="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="27" stopIfTrue="1">
-      <formula>$A33="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="29" stopIfTrue="1">
-      <formula>$A33="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="30" stopIfTrue="1">
-      <formula>$A33="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="32" stopIfTrue="1">
-      <formula>$A33="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="33" stopIfTrue="1">
-      <formula>$A33="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="35" stopIfTrue="1">
-      <formula>$A33="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:B34">
-    <cfRule type="expression" dxfId="101" priority="3" stopIfTrue="1">
-      <formula>$A33="comments"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:B34 F33:F34">
-    <cfRule type="expression" dxfId="100" priority="1" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A33, 14)="sensor_stream ", LEN($A33)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A33, 15)))), AND(LEFT($A33, 17)="sensor_statistic ", LEN($A33)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A33, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -6012,9 +5700,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6111,46 +5799,46 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B8" s="15">
         <v>1</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B9" s="15">
         <v>2</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B10" s="15">
         <v>3</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B11" s="15">
         <v>4</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -6171,7 +5859,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:H12">
-    <cfRule type="expression" dxfId="0" priority="100">
+    <cfRule type="expression" dxfId="98" priority="100">
       <formula>NOT($A12=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6229,7 +5917,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007102002</v>
+        <v>2007102327</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>
@@ -10065,348 +9753,348 @@
     <mergeCell ref="A83:B83"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="98" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="97" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="96" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="95" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="94" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="93" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="92" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="91" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="88" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="87" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="86" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="85" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="84" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="66" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="65" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="47" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="46" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="45" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="44" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="41" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="40" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="39" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="38" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="37" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="36" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated name of start button field plug-in
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF97591-7408-324A-9C93-B89469698648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3046DD4F-D556-1447-8F2C-315FFA976F26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27500" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2699,9 +2699,6 @@
     <t>Click/tap the button to start.</t>
   </si>
   <si>
-    <t>custom-start-button(key='none')</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -2837,6 +2834,9 @@
   </si>
   <si>
     <t>custom-timed-field-list(labels=${labels}, duration=10, required=1)</t>
+  </si>
+  <si>
+    <t>custom-button-to-advance(key='none')</t>
   </si>
 </sst>
 </file>
@@ -5007,7 +5007,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
@@ -5224,12 +5224,12 @@
         <v>148</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="N13" s="54" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -5241,15 +5241,15 @@
         <v>42</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5263,12 +5263,12 @@
         <v>400</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>401</v>
+        <v>445</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -5279,16 +5279,16 @@
         <v>375</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K17" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="L17" s="9" t="s">
         <v>402</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -5310,7 +5310,7 @@
         <v>379</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -5321,7 +5321,7 @@
         <v>381</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N20" s="9" t="s">
         <v>391</v>
@@ -5346,7 +5346,7 @@
         <v>148</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="N22" s="9" t="s">
         <v>319</v>
@@ -5360,7 +5360,7 @@
         <v>383</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -5368,7 +5368,7 @@
         <v>148</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="N24" s="9" t="s">
         <v>384</v>
@@ -5379,10 +5379,10 @@
         <v>148</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -5390,10 +5390,10 @@
         <v>148</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -5412,7 +5412,7 @@
         <v>385</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -5423,7 +5423,7 @@
         <v>388</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="289" x14ac:dyDescent="0.2">
@@ -5431,10 +5431,10 @@
         <v>42</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -5442,13 +5442,13 @@
         <v>374</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -5459,10 +5459,10 @@
         <v>389</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -5470,13 +5470,13 @@
         <v>374</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="F34" s="9" t="s">
         <v>433</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -5484,16 +5484,16 @@
         <v>374</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>438</v>
-      </c>
       <c r="K35" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -5501,13 +5501,13 @@
         <v>374</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C36" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>443</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -5515,13 +5515,13 @@
         <v>374</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="102" x14ac:dyDescent="0.2">
@@ -5532,10 +5532,10 @@
         <v>397</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -5543,13 +5543,13 @@
         <v>374</v>
       </c>
       <c r="B41" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>429</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="F41" s="9" t="s">
         <v>430</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007102327</v>
+        <v>2007102334</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Made field "labels_short" have fewer labels
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3046DD4F-D556-1447-8F2C-315FFA976F26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE2CC46-5EE5-934E-AE48-743AB36A1E35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27500" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2806,9 +2806,6 @@
     <t>labels_short</t>
   </si>
   <si>
-    <t>'Birds lay eggs.|Chickens have pencils.|Six is a shape.|A house has a door.|Football is a game.|Men can walk.|We eat paper.|Bees make bread.|Cars have tires.|Ball is a color.|Bees make honey.|A mouse has a door.|We eat food.|Red is a color.'</t>
-  </si>
-  <si>
     <t>not_endearly</t>
   </si>
   <si>
@@ -2837,6 +2834,9 @@
   </si>
   <si>
     <t>custom-button-to-advance(key='none')</t>
+  </si>
+  <si>
+    <t>'Birds lay eggs.|Chickens have pencils.|Six is a shape.|A house has a door.'</t>
   </si>
 </sst>
 </file>
@@ -5007,10 +5007,10 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5229,7 +5229,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="N13" s="54" t="s">
-        <v>435</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -5263,7 +5263,7 @@
         <v>400</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -5445,10 +5445,10 @@
         <v>422</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -5484,13 +5484,13 @@
         <v>374</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>436</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>437</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>401</v>
@@ -5501,13 +5501,13 @@
         <v>374</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C36" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>442</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -5521,7 +5521,7 @@
         <v>424</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="102" x14ac:dyDescent="0.2">
@@ -5917,7 +5917,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007102334</v>
+        <v>2007102347</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Simplified expression to retrieve time remaining
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE2CC46-5EE5-934E-AE48-743AB36A1E35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF76E5F-E3D2-F34A-B6F1-9D1801D256A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27500" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2756,9 +2756,6 @@
     <t>concat(${long_list_index}, '. ', ${long_list_row_label}, ' ', ${long_list_choice_label})</t>
   </si>
   <si>
-    <t>selected-at(item-at('|', ${long_list_data}, 0), 0)</t>
-  </si>
-  <si>
     <t>custom-timed-field-list(labels=${labels}, duration=20)</t>
   </si>
   <si>
@@ -2837,6 +2834,9 @@
   </si>
   <si>
     <t>'Birds lay eggs.|Chickens have pencils.|Six is a shape.|A house has a door.'</t>
+  </si>
+  <si>
+    <t>selected-at(${long_list_data}, 0)</t>
   </si>
 </sst>
 </file>
@@ -5010,7 +5010,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5224,12 +5224,12 @@
         <v>148</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="N13" s="54" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -5263,7 +5263,7 @@
         <v>400</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -5279,10 +5279,10 @@
         <v>375</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>401</v>
@@ -5310,7 +5310,7 @@
         <v>379</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>419</v>
+        <v>445</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -5442,13 +5442,13 @@
         <v>374</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -5459,10 +5459,10 @@
         <v>389</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -5470,13 +5470,13 @@
         <v>374</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="F34" s="9" t="s">
         <v>432</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -5484,13 +5484,13 @@
         <v>374</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>435</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>436</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>401</v>
@@ -5501,13 +5501,13 @@
         <v>374</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C36" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>441</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -5518,10 +5518,10 @@
         <v>407</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="102" x14ac:dyDescent="0.2">
@@ -5532,10 +5532,10 @@
         <v>397</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -5543,13 +5543,13 @@
         <v>374</v>
       </c>
       <c r="B41" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="F41" s="9" t="s">
         <v>429</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007102347</v>
+        <v>2007131750</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Performed touch-ups on sample form
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF76E5F-E3D2-F34A-B6F1-9D1801D256A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2977EE-F5BE-584C-A681-6E7D58B8B71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27500" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2721,10 +2721,6 @@
     <t>all_required</t>
   </si>
   <si>
-    <t>That was the main example. The following examples are not required so you can easily swipe between them and see how they work. In a real form, the field should be required, and it should be preceded by a &lt;em&gt;text&lt;/em&gt; field with the start-button field plug-in.
-The next several fields will show off several of the parameters you can use. Serveral different combinations of parameters are used, but these examples are not exhausted, so feel free to combine parameters in other ways.</t>
-  </si>
-  <si>
     <t>Number of rows. Subtract 1, because the first piece of data is for timing.</t>
   </si>
   <si>
@@ -2766,12 +2762,6 @@
   </si>
   <si>
     <t>This field will not block input after time runs out.</t>
-  </si>
-  <si>
-    <t>This field will only block input when each row has been completed.</t>
-  </si>
-  <si>
-    <t>custom-timed-field-list(labels=${labels}, duration=20, block=0)</t>
   </si>
   <si>
     <t>custom-timed-field-list(labels='Plot 1|Plot 2|Plot 3|Plot 4|Plot 5|Plot 6|Plot 7|Plot 8|Plot 9|Plot 10|Plot 11|Plot 12|Plot 13|Plot 14|Plot 15|', header='Plots', duration=20)</t>
@@ -2797,9 +2787,6 @@
     <t>This field has a 10-second timer, but the timer is not displayed. Input will be blocked after 10 seconds.</t>
   </si>
   <si>
-    <t>custom-timed-field-list(labels=${labels}, duration=20, disp=0)</t>
-  </si>
-  <si>
     <t>labels_short</t>
   </si>
   <si>
@@ -2812,24 +2799,12 @@
     <t>nochange</t>
   </si>
   <si>
-    <t>custom-timed-field-list(labels=${labels}, duration=20, advance=1, unit='ms')</t>
-  </si>
-  <si>
     <t>This field will auto-advance after time runs out. It also uses a different time unit.</t>
   </si>
   <si>
-    <t>In this field, the respondent cannot leave until time has run out, even if all fields have been completed. (This example field is required.)</t>
-  </si>
-  <si>
     <t>This field will disable a row after a choice has been selected. It will not block input after time runs out.</t>
   </si>
   <si>
-    <t>custom-timed-field-list(labels=${labels}, duration=20, nochange=1, block=0)</t>
-  </si>
-  <si>
-    <t>custom-timed-field-list(labels=${labels}, duration=10, required=1)</t>
-  </si>
-  <si>
     <t>custom-button-to-advance(key='none')</t>
   </si>
   <si>
@@ -2837,6 +2812,31 @@
   </si>
   <si>
     <t>selected-at(${long_list_data}, 0)</t>
+  </si>
+  <si>
+    <t>That was the main example. Most of the following examples are not required so you can easily swipe between them and see how they work. In a real form, the field should be required, and it should be preceded by a &lt;em&gt;text&lt;/em&gt; field with the button-to-advance field plug-in.
+The next several fields will show off several of the parameters you can use. Serveral different combinations of parameters are used, but these examples are not exhaustive, so feel free to combine parameters in other ways.</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, duration=10, disp=0)</t>
+  </si>
+  <si>
+    <t>In this field, the respondent cannot leave until time has run out, even if all fields have been completed. (This example field is required, and it only has four rows.)</t>
+  </si>
+  <si>
+    <t>This field will only block input when each row has been completed. (This field only has four rows.)</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels_short}, duration=10, required=1)</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, duration=10, nochange=1, block=0)</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, duration=10, block=0)</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels}, duration=10, advance=1, unit='ms')</t>
   </si>
 </sst>
 </file>
@@ -5007,7 +5007,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
@@ -5017,7 +5017,7 @@
   <cols>
     <col min="1" max="1" width="21.33203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42" style="10" customWidth="1"/>
     <col min="4" max="4" width="23" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="9" customWidth="1"/>
@@ -5224,12 +5224,12 @@
         <v>148</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="N13" s="54" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -5263,7 +5263,7 @@
         <v>400</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -5279,10 +5279,10 @@
         <v>375</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>401</v>
@@ -5310,7 +5310,7 @@
         <v>379</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -5321,7 +5321,7 @@
         <v>381</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N20" s="9" t="s">
         <v>391</v>
@@ -5346,7 +5346,7 @@
         <v>148</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="N22" s="9" t="s">
         <v>319</v>
@@ -5360,7 +5360,7 @@
         <v>383</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -5368,7 +5368,7 @@
         <v>148</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="N24" s="9" t="s">
         <v>384</v>
@@ -5379,10 +5379,10 @@
         <v>148</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -5390,10 +5390,10 @@
         <v>148</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -5412,7 +5412,7 @@
         <v>385</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -5423,10 +5423,10 @@
         <v>388</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="289" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="221" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>42</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>406</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>408</v>
+        <v>438</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -5442,13 +5442,13 @@
         <v>374</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -5459,10 +5459,10 @@
         <v>389</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>424</v>
+        <v>444</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -5470,13 +5470,13 @@
         <v>374</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -5484,13 +5484,13 @@
         <v>374</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>401</v>
@@ -5501,13 +5501,13 @@
         <v>374</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -5518,7 +5518,7 @@
         <v>407</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>423</v>
+        <v>441</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>442</v>
@@ -5532,10 +5532,10 @@
         <v>397</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -5543,13 +5543,13 @@
         <v>374</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007131750</v>
+        <v>2007141836</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Added appearances to labels
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2977EE-F5BE-584C-A681-6E7D58B8B71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E8C1F8-9F17-3D48-ADD5-A86714C7A0A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27500" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27480" yWindow="1220" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="448">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2755,38 +2755,18 @@
     <t>custom-timed-field-list(labels=${labels}, duration=20)</t>
   </si>
   <si>
-    <t>This field has no parameters defined other than the labels and the duration.</t>
-  </si>
-  <si>
     <t>auto_advance</t>
   </si>
   <si>
-    <t>This field will not block input after time runs out.</t>
-  </si>
-  <si>
-    <t>custom-timed-field-list(labels='Plot 1|Plot 2|Plot 3|Plot 4|Plot 5|Plot 6|Plot 7|Plot 8|Plot 9|Plot 10|Plot 11|Plot 12|Plot 13|Plot 14|Plot 15|', header='Plots', duration=20)</t>
-  </si>
-  <si>
-    <t>This is an example of a &lt;em&gt;select_multiple&lt;/em&gt; field.&lt;br&gt;
-&lt;br&gt;
-Select the crops you see in each plot.</t>
-  </si>
-  <si>
     <t>not_timed</t>
   </si>
   <si>
-    <t>This field is not timed.</t>
-  </si>
-  <si>
     <t>custom-timed-field-list(labels=${labels})</t>
   </si>
   <si>
     <t>no_disp</t>
   </si>
   <si>
-    <t>This field has a 10-second timer, but the timer is not displayed. Input will be blocked after 10 seconds.</t>
-  </si>
-  <si>
     <t>labels_short</t>
   </si>
   <si>
@@ -2797,12 +2777,6 @@
   </si>
   <si>
     <t>nochange</t>
-  </si>
-  <si>
-    <t>This field will auto-advance after time runs out. It also uses a different time unit.</t>
-  </si>
-  <si>
-    <t>This field will disable a row after a choice has been selected. It will not block input after time runs out.</t>
   </si>
   <si>
     <t>custom-button-to-advance(key='none')</t>
@@ -2821,15 +2795,6 @@
     <t>custom-timed-field-list(labels=${labels}, duration=10, disp=0)</t>
   </si>
   <si>
-    <t>In this field, the respondent cannot leave until time has run out, even if all fields have been completed. (This example field is required, and it only has four rows.)</t>
-  </si>
-  <si>
-    <t>This field will only block input when each row has been completed. (This field only has four rows.)</t>
-  </si>
-  <si>
-    <t>custom-timed-field-list(labels=${labels_short}, duration=10, required=1)</t>
-  </si>
-  <si>
     <t>custom-timed-field-list(labels=${labels}, duration=10, nochange=1, block=0)</t>
   </si>
   <si>
@@ -2837,6 +2802,65 @@
   </si>
   <si>
     <t>custom-timed-field-list(labels=${labels}, duration=10, advance=1, unit='ms')</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${labels_short}, duration=5, required=1)</t>
+  </si>
+  <si>
+    <t>plot_labels</t>
+  </si>
+  <si>
+    <t>custom-timed-field-list(labels=${plot_labels}, header='Plots', duration=20)</t>
+  </si>
+  <si>
+    <t>'Plot 1|Plot 2|Plot 3|Plot 4|Plot 5|Plot 6|Plot 7|Plot 8|Plot 9|Plot 10|Plot 11|Plot 12|Plot 13|Plot 14|Plot 15|'</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field has no parameters defined other than the labels and the duration.&lt;/p&gt;
+&lt;br&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-field-list(labels=&amp;#36;{labels}, duration=20)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field will auto-advance after time runs out. It also uses a different time unit.&lt;/p&gt;
+&lt;br&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-field-list(labels=&amp;#36;{labels}, duration=10, advance=1, unit='ms')&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field will not block input after time runs out.&lt;/p&gt;
+&lt;br&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-field-list(labels=&amp;#36;{labels}, duration=10, block=0)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field has a 10-second timer, but the timer is not displayed. Input will be blocked after 10 seconds.&lt;/p&gt;
+&lt;br&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-field-list(labels=&amp;#36;{labels}, duration=10, disp=0)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In this field, the respondent cannot leave until time has run out, even if all fields have been completed. (This example field is required, and it only has four rows.)&lt;/p&gt;
+&lt;br&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-field-list(labels=&amp;#36;{labels_short}, duration=10, endearly=0)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field will disable a row after a choice has been selected. It will not block input after time runs out.&lt;/p&gt;
+&lt;br&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-field-list(labels=&amp;#36;{labels}, duration=10, nochange=1, block=0)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field will only block input when each row has been completed. (This field only has four rows.)&lt;/p&gt;
+&lt;br&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-field-list(labels=&amp;#36;{labels_short}, duration=5, required=1)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This is an example of a &lt;em&gt;select_multiple&lt;/em&gt; field.&lt;br&gt;
+&lt;br&gt;
+Select the crops you see in each plot.&lt;/p&gt;
+&lt;br&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-field-list(labels=&amp;#36;{plot_labels}, header='Plots', duration=20)&lt;/code&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This field is not timed.&lt;/p&gt;
+&lt;br&gt;
+&lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-field-list(labels=&amp;#36;{labels})&lt;/code&gt;</t>
   </si>
 </sst>
 </file>
@@ -5004,13 +5028,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W41"/>
+  <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5224,82 +5248,84 @@
         <v>148</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="N13" s="54" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="1:23" ht="255" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>403</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>405</v>
-      </c>
+      <c r="N14" s="54" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
-      <c r="K15" s="9" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:23" ht="187" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>435</v>
+        <v>405</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="9" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>374</v>
+        <v>96</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>375</v>
+        <v>399</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>418</v>
-      </c>
+        <v>427</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
       <c r="K17" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="L17" s="9" t="s">
+    </row>
+    <row r="18" spans="1:15" ht="136" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="L18" s="9" t="s">
         <v>402</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>377</v>
-      </c>
-      <c r="N18" s="9" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -5307,49 +5333,49 @@
         <v>148</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>148</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="N20" s="9" t="s">
+      <c r="N21" s="9" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+    <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B22" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="O21" s="9" t="s">
+      <c r="O22" s="9" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>411</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -5357,10 +5383,10 @@
         <v>148</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>383</v>
+        <v>411</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>412</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -5368,10 +5394,10 @@
         <v>148</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>415</v>
+        <v>383</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>384</v>
+        <v>412</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -5379,10 +5405,10 @@
         <v>148</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>413</v>
+        <v>384</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -5390,166 +5416,177 @@
         <v>148</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>380</v>
+        <v>410</v>
+      </c>
+      <c r="N27" s="9" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B29" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="N28" s="9" t="s">
+      <c r="N29" s="9" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="68" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+    <row r="30" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C30" s="10" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="221" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+    <row r="32" spans="1:15" ht="221" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B32" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>420</v>
-      </c>
       <c r="C32" s="10" t="s">
-        <v>433</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>374</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>389</v>
+        <v>419</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>421</v>
+        <v>440</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>374</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>427</v>
+        <v>389</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>374</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="K35" s="9" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>374</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>374</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="102" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
+      <c r="C38" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="170" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B40" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>423</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
+      <c r="C40" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>424</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>426</v>
+      <c r="B42" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -5917,7 +5954,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007141836</v>
+        <v>2007201911</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>

</xml_diff>

<commit_message>
Updated sample form with intro
</commit_message>
<xml_diff>
--- a/extras/sample-form/Timed field list.xlsx
+++ b/extras/sample-form/Timed field list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-field-list/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABECFE9-7C02-BB42-958B-A2B137092F77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FF3466-496F-044E-8244-406EC527E5D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27480" yWindow="1220" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27960" yWindow="700" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="450">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2861,6 +2861,12 @@
 &lt;code style="font-size:90%;color:#c7254e;background-color:#f9f2f4;border-radius:4px"&gt;custom-timed-field-list(labels=&amp;#36;{plot_labels}, header='Plots', duration=20)&lt;/code&gt;
 &lt;br&gt;
 &lt;p&gt;Select the crops you see in each plot.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>intro</t>
+  </si>
+  <si>
+    <t>This is the sample form for the &lt;a href="https://github.com/surveycto/timed-field-list/wiki/Timed-field-list-wiki" target="_blank"&gt;timed-field-list&lt;/a&gt; field plug-in. This sample form also uses the &lt;a href="https://github.com/surveycto/button-to-advance/blob/master/README.md" target="_blank"&gt;button-to-advance&lt;/a&gt; field plug-in. Click on those links to learn more about how to download and use those field plug-ins.</t>
   </si>
 </sst>
 </file>
@@ -5028,10 +5034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W42"/>
+  <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
@@ -5273,70 +5279,75 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:23" ht="187" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="170" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>403</v>
+        <v>448</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>405</v>
+        <v>449</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>448</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
-      <c r="K16" s="9" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:15" ht="187" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="9" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="136" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>374</v>
+        <v>96</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>375</v>
+        <v>399</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>438</v>
+        <v>400</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>418</v>
-      </c>
+        <v>427</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
       <c r="K18" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="L18" s="9" t="s">
+    </row>
+    <row r="19" spans="1:15" ht="136" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="L19" s="9" t="s">
         <v>402</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>377</v>
-      </c>
-      <c r="N19" s="9" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -5344,49 +5355,49 @@
         <v>148</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>148</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="N21" s="9" t="s">
+      <c r="N22" s="9" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+    <row r="23" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B23" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="O22" s="9" t="s">
+      <c r="O23" s="9" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>411</v>
-      </c>
-      <c r="N23" s="9" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -5394,10 +5405,10 @@
         <v>148</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>383</v>
+        <v>411</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>412</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -5405,10 +5416,10 @@
         <v>148</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>415</v>
+        <v>383</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>384</v>
+        <v>412</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -5416,10 +5427,10 @@
         <v>148</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>413</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -5427,65 +5438,62 @@
         <v>148</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>380</v>
+        <v>410</v>
+      </c>
+      <c r="N28" s="9" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="N29" s="9" t="s">
+      <c r="N30" s="9" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="68" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+    <row r="31" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C31" s="10" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="272" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="1:11" ht="272" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B33" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C33" s="10" t="s">
         <v>446</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="136" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>419</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="136" x14ac:dyDescent="0.2">
@@ -5493,58 +5501,58 @@
         <v>374</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>389</v>
+        <v>419</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>374</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>422</v>
+        <v>389</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="170" x14ac:dyDescent="0.2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>374</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>374</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>431</v>
+        <v>425</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="153" x14ac:dyDescent="0.2">
@@ -5552,40 +5560,54 @@
         <v>374</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F39" s="9" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="170" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
+    <row r="41" spans="1:11" ht="170" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B41" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C41" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F41" s="9" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="102" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
+    <row r="43" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C43" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="F42" s="9" t="s">
+      <c r="F43" s="9" t="s">
         <v>421</v>
       </c>
     </row>
@@ -5954,7 +5976,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007201917</v>
+        <v>2007202225</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>367</v>
@@ -6546,7 +6568,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>102</v>
       </c>

</xml_diff>